<commit_message>
Modify ShelfController and ShelfExecutor func_inputs
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
   <si>
     <t>_Addr</t>
   </si>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,9 +606,6 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="F4" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
Create RackController to loop through ShelfController with ShelfNo.
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
   <si>
     <t>_Addr</t>
   </si>
@@ -187,6 +187,18 @@
   </si>
   <si>
     <t>shelf_reg_size</t>
+  </si>
+  <si>
+    <t>shelf_no_addr</t>
+  </si>
+  <si>
+    <t>shelf_reg_size_addr</t>
+  </si>
+  <si>
+    <t>D28001</t>
+  </si>
+  <si>
+    <t>D28002</t>
   </si>
 </sst>
 </file>
@@ -238,7 +250,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,599 +533,613 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>10</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3">
         <v>10000</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>200</v>
       </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="1">
+      <c r="H4" s="1">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="1">
+      <c r="H5" s="1">
         <v>8</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="1">
         <v>9</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+      <c r="I6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="1">
         <v>15</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+      <c r="I7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="1">
+      <c r="H8" s="1">
         <v>30</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="1">
         <v>31</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
+      <c r="I9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="1">
         <v>31.1</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+      <c r="I10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="1">
+      <c r="H11" s="1">
         <v>50</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="1">
         <v>51</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+      <c r="I12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="1">
         <v>51.1</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+      <c r="I13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="1">
         <v>51.2</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+      <c r="I14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="1">
+      <c r="H15" s="1">
         <v>52</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="1">
+      <c r="H16" s="1">
         <v>54</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="1">
+      <c r="H17" s="1">
         <v>56</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="1">
+      <c r="H18" s="1">
         <v>58</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="1">
+      <c r="H19" s="1">
         <v>100</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="1">
         <v>101</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+      <c r="I20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J20" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="1">
         <v>101.1</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H21" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+      <c r="I21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="1">
         <v>101.2</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H22" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+      <c r="I22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="1">
+      <c r="H23" s="1">
         <v>102</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="1">
+      <c r="H24" s="1">
         <v>104</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="1">
+      <c r="H25" s="1">
         <v>106</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1">
+      <c r="H26" s="1">
         <v>108</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H26" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="1">
         <v>109</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H27" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
+      <c r="I27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J27" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="1">
+      <c r="H28" s="1">
         <v>150</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="1">
         <v>151</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H29" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
+      <c r="I29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J29" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="1">
         <v>151.1</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H30" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
+      <c r="I30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J30" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" s="1">
         <v>151.19999999999999</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H31" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+      <c r="I31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J31" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="1">
+      <c r="H32" s="1">
         <v>152</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
         <v>31</v>
       </c>
-      <c r="F33" s="1">
+      <c r="H33" s="1">
         <v>154</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="1">
+      <c r="H34" s="1">
         <v>156</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="1">
+      <c r="H35" s="1">
         <v>158</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H35" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
+      <c r="J35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F36" s="1">
+      <c r="G36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" s="1">
         <v>159</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H36" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="H37" s="1"/>
+      <c r="I36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J36" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="J37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modify all functions to take work on WORD instead of REAL
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="60">
   <si>
     <t>_Addr</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>D28002</t>
+  </si>
+  <si>
+    <t>ARRAY [3] OF WORD</t>
+  </si>
+  <si>
+    <t>[3(0)]</t>
   </si>
 </sst>
 </file>
@@ -533,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,9 +557,10 @@
     <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>51</v>
       </c>
@@ -585,7 +592,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>10</v>
       </c>
@@ -613,8 +620,17 @@
       <c r="J2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>1</v>
       </c>
@@ -630,8 +646,17 @@
       <c r="J3" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>2</v>
       </c>
@@ -639,27 +664,45 @@
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
         <v>8</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>4</v>
       </c>
@@ -667,16 +710,25 @@
         <v>37</v>
       </c>
       <c r="H6" s="1">
+        <v>6</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
         <v>9</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>5</v>
       </c>
@@ -684,30 +736,48 @@
         <v>37</v>
       </c>
       <c r="H7" s="1">
+        <v>10</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
         <v>15</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>6</v>
       </c>
       <c r="H8" s="1">
+        <v>15</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
         <v>30</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>7</v>
       </c>
@@ -715,16 +785,25 @@
         <v>37</v>
       </c>
       <c r="H9" s="1">
+        <v>16</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
         <v>31</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J9" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N9" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>8</v>
       </c>
@@ -732,30 +811,48 @@
         <v>37</v>
       </c>
       <c r="H10" s="1">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
         <v>31.1</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="1">
+        <v>30</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
         <v>50</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>10</v>
       </c>
@@ -763,16 +860,25 @@
         <v>37</v>
       </c>
       <c r="H12" s="1">
+        <v>31</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
         <v>51</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J12" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N12" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>11</v>
       </c>
@@ -780,16 +886,25 @@
         <v>37</v>
       </c>
       <c r="H13" s="1">
+        <v>31.1</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
         <v>51.1</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J13" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N13" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
         <v>12</v>
       </c>
@@ -797,86 +912,140 @@
         <v>37</v>
       </c>
       <c r="H14" s="1">
+        <v>31.2</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
         <v>51.2</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N14" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>13</v>
       </c>
       <c r="H15" s="1">
+        <v>32</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
         <v>52</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>14</v>
       </c>
       <c r="H16" s="1">
+        <v>33</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
         <v>54</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>15</v>
       </c>
       <c r="H17" s="1">
+        <v>34</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
         <v>56</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="1">
+        <v>35</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
         <v>58</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>17</v>
       </c>
       <c r="H19" s="1">
+        <v>50</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
         <v>100</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>18</v>
       </c>
@@ -884,16 +1053,25 @@
         <v>37</v>
       </c>
       <c r="H20" s="1">
+        <v>51</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
         <v>101</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J20" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N20" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>19</v>
       </c>
@@ -901,16 +1079,25 @@
         <v>37</v>
       </c>
       <c r="H21" s="1">
+        <v>51.1</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
         <v>101.1</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J21" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N21" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>20</v>
       </c>
@@ -918,72 +1105,117 @@
         <v>37</v>
       </c>
       <c r="H22" s="1">
+        <v>51.2</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
         <v>101.2</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J22" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N22" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>21</v>
       </c>
       <c r="H23" s="1">
+        <v>52</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
         <v>102</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>22</v>
       </c>
       <c r="H24" s="1">
+        <v>53</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
         <v>104</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="M24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="N24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>23</v>
       </c>
       <c r="H25" s="1">
+        <v>54</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
         <v>106</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="N25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
         <v>24</v>
       </c>
       <c r="H26" s="1">
+        <v>55</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
         <v>108</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J26" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>25</v>
       </c>
@@ -991,30 +1223,48 @@
         <v>37</v>
       </c>
       <c r="H27" s="1">
+        <v>56</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
         <v>109</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J27" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N27" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>26</v>
       </c>
       <c r="H28" s="1">
+        <v>70</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
         <v>150</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>27</v>
       </c>
@@ -1022,16 +1272,25 @@
         <v>37</v>
       </c>
       <c r="H29" s="1">
+        <v>71</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
         <v>151</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J29" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N29" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>28</v>
       </c>
@@ -1039,16 +1298,25 @@
         <v>37</v>
       </c>
       <c r="H30" s="1">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
         <v>151.1</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J30" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N30" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>29</v>
       </c>
@@ -1056,72 +1324,117 @@
         <v>37</v>
       </c>
       <c r="H31" s="1">
+        <v>71.2</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1">
         <v>151.19999999999999</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J31" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N31" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>30</v>
       </c>
       <c r="H32" s="1">
+        <v>72</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
         <v>152</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="M32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="N32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
         <v>31</v>
       </c>
       <c r="H33" s="1">
+        <v>73</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
         <v>154</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="M33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="N33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
         <v>32</v>
       </c>
       <c r="H34" s="1">
+        <v>74</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
         <v>156</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="M34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="N34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
         <v>33</v>
       </c>
       <c r="H35" s="1">
+        <v>75</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1">
         <v>158</v>
       </c>
-      <c r="I35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J35" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
         <v>34</v>
       </c>
@@ -1129,16 +1442,25 @@
         <v>37</v>
       </c>
       <c r="H36" s="1">
+        <v>76</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1">
         <v>159</v>
       </c>
-      <c r="I36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J36" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="M36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N36" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
       <c r="J37" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify script and template to create sensor_variable(s)
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shibin.hoo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shibin.hoo\Documents\GitHub\Ellemento\rack_control\plc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="5715"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="5715" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
     <sheet name="Shelf" sheetId="1" r:id="rId2"/>
+    <sheet name="Shelf Sensor" sheetId="3" r:id="rId3"/>
+    <sheet name="Sensor Data" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="66">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -175,6 +177,54 @@
   </si>
   <si>
     <t>[3(0)]</t>
+  </si>
+  <si>
+    <t>shelf_sensor_reg_size</t>
+  </si>
+  <si>
+    <t>wPres0</t>
+  </si>
+  <si>
+    <t>wPres1</t>
+  </si>
+  <si>
+    <t>wPres2</t>
+  </si>
+  <si>
+    <t>wTemp0</t>
+  </si>
+  <si>
+    <t>wTemp1</t>
+  </si>
+  <si>
+    <t>wTemp2</t>
+  </si>
+  <si>
+    <t>aTemp</t>
+  </si>
+  <si>
+    <t>aRH</t>
+  </si>
+  <si>
+    <t>aCO2</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>warn_u</t>
+  </si>
+  <si>
+    <t>warn_l</t>
+  </si>
+  <si>
+    <t>err_u</t>
+  </si>
+  <si>
+    <t>err_l</t>
   </si>
 </sst>
 </file>
@@ -511,13 +561,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -562,6 +612,14 @@
       </c>
       <c r="D3">
         <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -588,7 +646,7 @@
   <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,4 +1413,174 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>12000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove snsr_sX_wTemp2 from template and generate global_variable_table
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="5715" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="5715"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t>wTemp1</t>
-  </si>
-  <si>
-    <t>wTemp2</t>
   </si>
   <si>
     <t>aTemp</t>
@@ -564,7 +561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -619,7 +616,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4">
         <v>28003</v>
@@ -628,12 +625,12 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>28004</v>
@@ -1440,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,22 +1487,17 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1517,7 +1509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1539,7 +1531,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1550,7 +1542,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1561,7 +1553,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1572,7 +1564,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1583,7 +1575,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1594,7 +1586,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Change sensor_data_table (by sensor_type, instead of shelf_no)
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="5715"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="5715" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>snsr_no</t>
+  </si>
+  <si>
+    <t>aFlow</t>
+  </si>
+  <si>
+    <t>shelf_sensor</t>
   </si>
 </sst>
 </file>
@@ -561,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1437,10 +1443,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,7 +1460,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1487,16 +1493,21 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Populate the list with general sensors.
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
     <sheet name="Shelf" sheetId="1" r:id="rId2"/>
-    <sheet name="Shelf Sensor" sheetId="3" r:id="rId3"/>
+    <sheet name="Sensor List" sheetId="3" r:id="rId3"/>
     <sheet name="Sensor Data" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="167">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -194,15 +194,6 @@
     <t>wTemp1</t>
   </si>
   <si>
-    <t>aTemp</t>
-  </si>
-  <si>
-    <t>aRH</t>
-  </si>
-  <si>
-    <t>aCO2</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -227,10 +218,316 @@
     <t>snsr_no</t>
   </si>
   <si>
-    <t>aFlow</t>
-  </si>
-  <si>
     <t>shelf_sensor</t>
+  </si>
+  <si>
+    <t>general_sensor</t>
+  </si>
+  <si>
+    <t>wFlow0</t>
+  </si>
+  <si>
+    <t>aFlow0</t>
+  </si>
+  <si>
+    <t>wFlow1</t>
+  </si>
+  <si>
+    <t>aFlow2</t>
+  </si>
+  <si>
+    <t>aCO2_0</t>
+  </si>
+  <si>
+    <t>aRH_0</t>
+  </si>
+  <si>
+    <t>aTemp0</t>
+  </si>
+  <si>
+    <t>aFlow1</t>
+  </si>
+  <si>
+    <t>aFlow3</t>
+  </si>
+  <si>
+    <t>aFlow4</t>
+  </si>
+  <si>
+    <t>aFlow5</t>
+  </si>
+  <si>
+    <t>aFlow6</t>
+  </si>
+  <si>
+    <t>aFlow7</t>
+  </si>
+  <si>
+    <t>aFlow8</t>
+  </si>
+  <si>
+    <t>aFlow9</t>
+  </si>
+  <si>
+    <t>aFlow10</t>
+  </si>
+  <si>
+    <t>aFlow11</t>
+  </si>
+  <si>
+    <t>aFlow12</t>
+  </si>
+  <si>
+    <t>aFlow13</t>
+  </si>
+  <si>
+    <t>aFlow14</t>
+  </si>
+  <si>
+    <t>aFlow15</t>
+  </si>
+  <si>
+    <t>aFlow16</t>
+  </si>
+  <si>
+    <t>aFlow17</t>
+  </si>
+  <si>
+    <t>aFlow18</t>
+  </si>
+  <si>
+    <t>aFlow19</t>
+  </si>
+  <si>
+    <t>aFlow20</t>
+  </si>
+  <si>
+    <t>aFlow21</t>
+  </si>
+  <si>
+    <t>aFlow22</t>
+  </si>
+  <si>
+    <t>aFlow23</t>
+  </si>
+  <si>
+    <t>aFlow24</t>
+  </si>
+  <si>
+    <t>aTemp1</t>
+  </si>
+  <si>
+    <t>aTemp2</t>
+  </si>
+  <si>
+    <t>aTemp3</t>
+  </si>
+  <si>
+    <t>aTemp4</t>
+  </si>
+  <si>
+    <t>aTemp5</t>
+  </si>
+  <si>
+    <t>aTemp6</t>
+  </si>
+  <si>
+    <t>aTemp7</t>
+  </si>
+  <si>
+    <t>aTemp8</t>
+  </si>
+  <si>
+    <t>aTemp9</t>
+  </si>
+  <si>
+    <t>aTemp10</t>
+  </si>
+  <si>
+    <t>aTemp11</t>
+  </si>
+  <si>
+    <t>aTemp12</t>
+  </si>
+  <si>
+    <t>aTemp13</t>
+  </si>
+  <si>
+    <t>aTemp14</t>
+  </si>
+  <si>
+    <t>aTemp15</t>
+  </si>
+  <si>
+    <t>aTemp16</t>
+  </si>
+  <si>
+    <t>aTemp17</t>
+  </si>
+  <si>
+    <t>aTemp18</t>
+  </si>
+  <si>
+    <t>aTemp19</t>
+  </si>
+  <si>
+    <t>aTemp20</t>
+  </si>
+  <si>
+    <t>aTemp21</t>
+  </si>
+  <si>
+    <t>aTemp22</t>
+  </si>
+  <si>
+    <t>aTemp23</t>
+  </si>
+  <si>
+    <t>aTemp24</t>
+  </si>
+  <si>
+    <t>aCO2_1</t>
+  </si>
+  <si>
+    <t>aCO2_2</t>
+  </si>
+  <si>
+    <t>aCO2_3</t>
+  </si>
+  <si>
+    <t>aCO2_4</t>
+  </si>
+  <si>
+    <t>aCO2_5</t>
+  </si>
+  <si>
+    <t>aCO2_6</t>
+  </si>
+  <si>
+    <t>aCO2_7</t>
+  </si>
+  <si>
+    <t>aCO2_8</t>
+  </si>
+  <si>
+    <t>aCO2_9</t>
+  </si>
+  <si>
+    <t>aCO2_10</t>
+  </si>
+  <si>
+    <t>aCO2_11</t>
+  </si>
+  <si>
+    <t>aCO2_12</t>
+  </si>
+  <si>
+    <t>aCO2_13</t>
+  </si>
+  <si>
+    <t>aCO2_14</t>
+  </si>
+  <si>
+    <t>aCO2_15</t>
+  </si>
+  <si>
+    <t>aCO2_16</t>
+  </si>
+  <si>
+    <t>aCO2_17</t>
+  </si>
+  <si>
+    <t>aCO2_18</t>
+  </si>
+  <si>
+    <t>aCO2_19</t>
+  </si>
+  <si>
+    <t>aCO2_20</t>
+  </si>
+  <si>
+    <t>aCO2_21</t>
+  </si>
+  <si>
+    <t>aCO2_22</t>
+  </si>
+  <si>
+    <t>aCO2_23</t>
+  </si>
+  <si>
+    <t>aCO2_24</t>
+  </si>
+  <si>
+    <t>aRH_1</t>
+  </si>
+  <si>
+    <t>aRH_2</t>
+  </si>
+  <si>
+    <t>aRH_3</t>
+  </si>
+  <si>
+    <t>aRH_4</t>
+  </si>
+  <si>
+    <t>aRH_5</t>
+  </si>
+  <si>
+    <t>aRH_6</t>
+  </si>
+  <si>
+    <t>aRH_7</t>
+  </si>
+  <si>
+    <t>aRH_8</t>
+  </si>
+  <si>
+    <t>aRH_9</t>
+  </si>
+  <si>
+    <t>aRH_10</t>
+  </si>
+  <si>
+    <t>aRH_11</t>
+  </si>
+  <si>
+    <t>aRH_12</t>
+  </si>
+  <si>
+    <t>aRH_13</t>
+  </si>
+  <si>
+    <t>aRH_14</t>
+  </si>
+  <si>
+    <t>aRH_15</t>
+  </si>
+  <si>
+    <t>aRH_16</t>
+  </si>
+  <si>
+    <t>aRH_17</t>
+  </si>
+  <si>
+    <t>aRH_18</t>
+  </si>
+  <si>
+    <t>aRH_19</t>
+  </si>
+  <si>
+    <t>aRH_20</t>
+  </si>
+  <si>
+    <t>aRH_21</t>
+  </si>
+  <si>
+    <t>aRH_22</t>
+  </si>
+  <si>
+    <t>aRH_23</t>
+  </si>
+  <si>
+    <t>aRH_24</t>
   </si>
 </sst>
 </file>
@@ -622,7 +919,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B4">
         <v>28003</v>
@@ -636,7 +933,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B5">
         <v>28004</v>
@@ -1443,76 +1740,561 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12000</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>55</v>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1542,7 +2324,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1553,7 +2335,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1564,7 +2346,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1575,7 +2357,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1586,7 +2368,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1597,7 +2379,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Update snsr_no in template. Tested
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="168">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -528,6 +528,9 @@
   </si>
   <si>
     <t>aRH_24</t>
+  </si>
+  <si>
+    <t>Number is udpated automatically.</t>
   </si>
 </sst>
 </file>
@@ -551,12 +554,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -571,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -582,6 +591,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,7 +875,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,8 +937,12 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
-        <v>80</v>
+      <c r="D4" s="4">
+        <f>D2*(COUNTA('Sensor List'!B:B)-1) + (COUNTA('Sensor List'!C:C)-1)</f>
+        <v>152</v>
+      </c>
+      <c r="F4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1743,7 +1757,7 @@
   <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Change constant_variable base_addr to D25000.
D28000 was actually used for data exchange. Clashed memory.
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="5715" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="5715"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +904,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>28001</v>
+        <v>25001</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -918,7 +918,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>28002</v>
+        <v>25002</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -932,7 +932,7 @@
         <v>62</v>
       </c>
       <c r="B4">
-        <v>28003</v>
+        <v>25003</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -950,7 +950,7 @@
         <v>61</v>
       </c>
       <c r="B5">
-        <v>28004</v>
+        <v>25004</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1756,8 +1756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update global_variable_template to create boolean instead of word for on/off data
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="5715" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="5712"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="158">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -486,6 +486,21 @@
   </si>
   <si>
     <t>m_PV_PosArr</t>
+  </si>
+  <si>
+    <t>hmi_tag</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>o_PV_PosArr</t>
+  </si>
+  <si>
+    <t>o_lightIntensity</t>
+  </si>
+  <si>
+    <t>o_lightOn</t>
   </si>
 </sst>
 </file>
@@ -832,18 +847,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -857,7 +872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -871,7 +886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -882,10 +897,10 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -903,7 +918,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -917,14 +932,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -940,24 +955,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -973,8 +989,11 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10000</v>
       </c>
@@ -994,7 +1013,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1009,7 +1028,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -1024,7 +1043,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>139</v>
       </c>
@@ -1039,42 +1058,42 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="C6" s="1">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1">
         <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="1">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="1">
-        <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>1</v>
@@ -1084,102 +1103,117 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="1">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="1">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="1">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="1">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C13" s="1">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="1">
+        <v>16</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="F14" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="1">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>145</v>
-      </c>
-      <c r="C12" s="1">
-        <v>30</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C13" s="1">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="1">
-        <v>36</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>147</v>
-      </c>
       <c r="C15" s="1">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
@@ -1187,320 +1221,377 @@
       <c r="E15" s="1">
         <v>0</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16" s="1">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="1">
+        <v>23</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1">
+        <v>26</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="1">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>152</v>
       </c>
-      <c r="C16" s="1">
-        <v>38</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C20" s="1">
+        <v>28</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17" s="1">
-        <v>50</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="F20" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="1">
+        <v>31</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
         <v>0</v>
       </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>149</v>
-      </c>
-      <c r="C18" s="1">
-        <v>51</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="1">
-        <v>54</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>150</v>
-      </c>
-      <c r="C20" s="1">
-        <v>55</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E22" s="1"/>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="1">
+        <v>32</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E23" s="1"/>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="1">
+        <v>33</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E24" s="1"/>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="G24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E25" s="1"/>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="G25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E26" s="1"/>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="G26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="E27" s="1"/>
       <c r="G27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="E28" s="1"/>
       <c r="G28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="E29" s="1"/>
       <c r="G29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="E30" s="1"/>
       <c r="G30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="E31" s="1"/>
       <c r="G31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="E32" s="1"/>
       <c r="G32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E33" s="1"/>
       <c r="G33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E34" s="1"/>
       <c r="G34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E35" s="1"/>
       <c r="G35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E36" s="1"/>
       <c r="G36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E81" s="1"/>
     </row>
   </sheetData>
@@ -1517,14 +1608,14 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1535,7 +1626,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>12000</v>
       </c>
@@ -1546,7 +1637,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>22</v>
       </c>
@@ -1554,7 +1645,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>23</v>
       </c>
@@ -1562,7 +1653,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>24</v>
       </c>
@@ -1570,7 +1661,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>25</v>
       </c>
@@ -1578,487 +1669,487 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C66" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C68" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C70" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C73" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C76" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C77" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C78" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C80" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C85" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C86" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C87" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C89" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C90" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C91" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C92" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C93" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C94" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C95" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C96" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C102" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C103" t="s">
         <v>137</v>
       </c>
@@ -2077,12 +2168,12 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2093,7 +2184,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2104,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -2115,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2126,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -2137,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2148,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Modify global_variable_generator.py to generate hmi_tag.csv as well
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="5712" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5715" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -851,14 +851,14 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -872,7 +872,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -886,7 +886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -900,7 +900,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -918,7 +918,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -932,14 +932,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -955,25 +955,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -993,7 +993,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10000</v>
       </c>
@@ -1013,7 +1013,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>139</v>
       </c>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>148</v>
       </c>
@@ -1073,7 +1073,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>149</v>
       </c>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>18</v>
       </c>
@@ -1103,7 +1103,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>150</v>
       </c>
@@ -1118,7 +1118,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>140</v>
       </c>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>141</v>
       </c>
@@ -1154,7 +1154,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>142</v>
       </c>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>143</v>
       </c>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>144</v>
       </c>
@@ -1208,7 +1208,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>145</v>
       </c>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>146</v>
       </c>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>147</v>
       </c>
@@ -1298,7 +1298,7 @@
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>152</v>
       </c>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>156</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="G21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>157</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="G22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>155</v>
       </c>
@@ -1373,225 +1373,225 @@
       <c r="G23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E27" s="1"/>
       <c r="G27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E28" s="1"/>
       <c r="G28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E29" s="1"/>
       <c r="G29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E30" s="1"/>
       <c r="G30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E31" s="1"/>
       <c r="G31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E32" s="1"/>
       <c r="G32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E33" s="1"/>
       <c r="G33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E34" s="1"/>
       <c r="G34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E35" s="1"/>
       <c r="G35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E36" s="1"/>
       <c r="G36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E81" s="1"/>
     </row>
   </sheetData>
@@ -1608,14 +1608,14 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12000</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>22</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>23</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>24</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>25</v>
       </c>
@@ -1669,487 +1669,487 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C100" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C101" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C103" t="s">
         <v>137</v>
       </c>
@@ -2164,16 +2164,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Update global_variable_generator to include pump variables
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5715" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5715" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
     <sheet name="Shelf" sheetId="1" r:id="rId2"/>
     <sheet name="Sensor List" sheetId="3" r:id="rId3"/>
     <sheet name="Sensor Data" sheetId="4" r:id="rId4"/>
+    <sheet name="Pump" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="172">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -501,6 +502,48 @@
   </si>
   <si>
     <t>o_lightOn</t>
+  </si>
+  <si>
+    <t>ARRAY [4] OF BOOL</t>
+  </si>
+  <si>
+    <t>[4(FALSE)]</t>
+  </si>
+  <si>
+    <t>pump_e_OnArr</t>
+  </si>
+  <si>
+    <t>pump_e_FlowOrRpm</t>
+  </si>
+  <si>
+    <t>pump_e_FlowSetArr</t>
+  </si>
+  <si>
+    <t>pump_e_RpmSetArr</t>
+  </si>
+  <si>
+    <t>pump_e_RpmValArr</t>
+  </si>
+  <si>
+    <t>pump_e_ValveOnArr</t>
+  </si>
+  <si>
+    <t>pump_h_Mode</t>
+  </si>
+  <si>
+    <t>pump_h_OnArr</t>
+  </si>
+  <si>
+    <t>pump_h_FlowSetArr</t>
+  </si>
+  <si>
+    <t>pump_h_RpmSetArr</t>
+  </si>
+  <si>
+    <t>pump_h_RpmValArr</t>
+  </si>
+  <si>
+    <t>pump_h_ValveOnArr</t>
   </si>
 </sst>
 </file>
@@ -955,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,4 +2296,236 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" t="s">
+        <v>159</v>
+      </c>
+      <c r="F13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modify global_variable_generator addr_offset to be relative
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5715" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5715" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -891,7 +891,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +999,7 @@
   <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,7 +1044,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -1076,7 +1076,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
@@ -1106,7 +1106,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
@@ -1121,7 +1121,7 @@
         <v>149</v>
       </c>
       <c r="C7" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>19</v>
@@ -1136,7 +1136,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>1</v>
@@ -1151,7 +1151,7 @@
         <v>150</v>
       </c>
       <c r="C9" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
@@ -1166,7 +1166,7 @@
         <v>140</v>
       </c>
       <c r="C10" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
@@ -1184,7 +1184,7 @@
         <v>141</v>
       </c>
       <c r="C11" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>3</v>
@@ -1202,7 +1202,7 @@
         <v>142</v>
       </c>
       <c r="C12" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>3</v>
@@ -1220,7 +1220,7 @@
         <v>143</v>
       </c>
       <c r="C13" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>2</v>
@@ -1238,7 +1238,7 @@
         <v>144</v>
       </c>
       <c r="C14" s="1">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>19</v>
@@ -1256,7 +1256,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="1">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
@@ -1274,7 +1274,7 @@
         <v>145</v>
       </c>
       <c r="C16" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>2</v>
@@ -1292,7 +1292,7 @@
         <v>146</v>
       </c>
       <c r="C17" s="1">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>19</v>
@@ -1310,7 +1310,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="1">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1</v>
@@ -1328,7 +1328,7 @@
         <v>147</v>
       </c>
       <c r="C19" s="1">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>3</v>
@@ -1346,7 +1346,7 @@
         <v>152</v>
       </c>
       <c r="C20" s="1">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>19</v>
@@ -1364,7 +1364,7 @@
         <v>156</v>
       </c>
       <c r="C21" s="1">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>1</v>
@@ -1383,7 +1383,7 @@
         <v>157</v>
       </c>
       <c r="C22" s="1">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>3</v>
@@ -1402,7 +1402,7 @@
         <v>155</v>
       </c>
       <c r="C23" s="1">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>19</v>
@@ -2207,7 +2207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2302,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2343,7 +2343,7 @@
         <v>160</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -2372,7 +2372,7 @@
         <v>162</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
@@ -2386,7 +2386,7 @@
         <v>163</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -2400,7 +2400,7 @@
         <v>164</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
@@ -2414,7 +2414,7 @@
         <v>165</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>158</v>
@@ -2428,7 +2428,7 @@
         <v>166</v>
       </c>
       <c r="C8">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>1</v>
@@ -2445,7 +2445,7 @@
         <v>167</v>
       </c>
       <c r="C9">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>2</v>
@@ -2462,7 +2462,7 @@
         <v>168</v>
       </c>
       <c r="C10">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>19</v>
@@ -2479,7 +2479,7 @@
         <v>169</v>
       </c>
       <c r="C11">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>19</v>
@@ -2496,7 +2496,7 @@
         <v>170</v>
       </c>
       <c r="C12">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>19</v>
@@ -2513,7 +2513,7 @@
         <v>171</v>
       </c>
       <c r="C13">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>158</v>

</xml_diff>

<commit_message>
Add HMI_internal into global_variable_generator
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5715" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5715" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Sensor List" sheetId="3" r:id="rId3"/>
     <sheet name="Sensor Data" sheetId="4" r:id="rId4"/>
     <sheet name="Pump" sheetId="5" r:id="rId5"/>
+    <sheet name="HMI Internal" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="181">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -544,12 +545,43 @@
   </si>
   <si>
     <t>pump_h_ValveOnArr</t>
+  </si>
+  <si>
+    <t>PUMP_0_SELECTED</t>
+  </si>
+  <si>
+    <t>BIT</t>
+  </si>
+  <si>
+    <t>PUMP_1_SELECTED</t>
+  </si>
+  <si>
+    <t>PUMP_2_SELECTED</t>
+  </si>
+  <si>
+    <t>PUMP_CHECK</t>
+  </si>
+  <si>
+    <t>DUMMY_BIT</t>
+  </si>
+  <si>
+    <t>STRING</t>
+  </si>
+  <si>
+    <t>var_name</t>
+  </si>
+  <si>
+    <t>var_type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -593,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -608,6 +640,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2302,7 +2336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -2528,4 +2562,114 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update global_variable to contain IO_mapping
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5715" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5715" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,8 @@
     <sheet name="Sensor List" sheetId="3" r:id="rId3"/>
     <sheet name="Sensor Data" sheetId="4" r:id="rId4"/>
     <sheet name="Pump" sheetId="5" r:id="rId5"/>
-    <sheet name="HMI Internal" sheetId="7" r:id="rId6"/>
+    <sheet name="IO Mapping" sheetId="8" r:id="rId6"/>
+    <sheet name="HMI Internal" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="335">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -572,6 +573,468 @@
   </si>
   <si>
     <t>var_type</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s0_0</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s0_1</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s0_2</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s1_0</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s2_1</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s3_2</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s1_1</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s1_2</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s2_0</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s2_2</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s3_0</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s3_1</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s4_0</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s4_1</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s4_2</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s5_0</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s5_1</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s5_2</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s6_0</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s6_1</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s6_2</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s7_0</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s7_1</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s7_2</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s8_1</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s8_0</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s8_2</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s9_0</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s9_1</t>
+  </si>
+  <si>
+    <t>IO_waterPres_s9_2</t>
+  </si>
+  <si>
+    <t>D28002</t>
+  </si>
+  <si>
+    <t>D28004</t>
+  </si>
+  <si>
+    <t>D28006</t>
+  </si>
+  <si>
+    <t>D28008</t>
+  </si>
+  <si>
+    <t>D28010</t>
+  </si>
+  <si>
+    <t>D28012</t>
+  </si>
+  <si>
+    <t>D28014</t>
+  </si>
+  <si>
+    <t>D28016</t>
+  </si>
+  <si>
+    <t>D28022</t>
+  </si>
+  <si>
+    <t>D28024</t>
+  </si>
+  <si>
+    <t>D28026</t>
+  </si>
+  <si>
+    <t>D28028</t>
+  </si>
+  <si>
+    <t>D28030</t>
+  </si>
+  <si>
+    <t>D28032</t>
+  </si>
+  <si>
+    <t>D28034</t>
+  </si>
+  <si>
+    <t>D28036</t>
+  </si>
+  <si>
+    <t>D28042</t>
+  </si>
+  <si>
+    <t>D28044</t>
+  </si>
+  <si>
+    <t>D28046</t>
+  </si>
+  <si>
+    <t>D28048</t>
+  </si>
+  <si>
+    <t>D28050</t>
+  </si>
+  <si>
+    <t>D28052</t>
+  </si>
+  <si>
+    <t>D28054</t>
+  </si>
+  <si>
+    <t>D28056</t>
+  </si>
+  <si>
+    <t>D28062</t>
+  </si>
+  <si>
+    <t>D28064</t>
+  </si>
+  <si>
+    <t>D28066</t>
+  </si>
+  <si>
+    <t>D28068</t>
+  </si>
+  <si>
+    <t>D28070</t>
+  </si>
+  <si>
+    <t>D28072</t>
+  </si>
+  <si>
+    <t>IO_flowmeter_0</t>
+  </si>
+  <si>
+    <t>IO_flowmeter_1</t>
+  </si>
+  <si>
+    <t>IO_propValve_s0_0</t>
+  </si>
+  <si>
+    <t>IO_propValve_s0_1</t>
+  </si>
+  <si>
+    <t>IO_propValve_s0_2</t>
+  </si>
+  <si>
+    <t>IO_propValve_s1_0</t>
+  </si>
+  <si>
+    <t>IO_propValve_s1_1</t>
+  </si>
+  <si>
+    <t>IO_propValve_s1_2</t>
+  </si>
+  <si>
+    <t>IO_propValve_s2_0</t>
+  </si>
+  <si>
+    <t>IO_propValve_s2_1</t>
+  </si>
+  <si>
+    <t>IO_propValve_s2_2</t>
+  </si>
+  <si>
+    <t>IO_propValve_s3_0</t>
+  </si>
+  <si>
+    <t>IO_propValve_s3_1</t>
+  </si>
+  <si>
+    <t>IO_propValve_s3_2</t>
+  </si>
+  <si>
+    <t>IO_propValve_s4_0</t>
+  </si>
+  <si>
+    <t>IO_propValve_s4_1</t>
+  </si>
+  <si>
+    <t>IO_propValve_s4_2</t>
+  </si>
+  <si>
+    <t>IO_propValve_s5_0</t>
+  </si>
+  <si>
+    <t>IO_propValve_s5_1</t>
+  </si>
+  <si>
+    <t>IO_propValve_s5_2</t>
+  </si>
+  <si>
+    <t>IO_propValve_s6_0</t>
+  </si>
+  <si>
+    <t>IO_propValve_s6_1</t>
+  </si>
+  <si>
+    <t>IO_propValve_s6_2</t>
+  </si>
+  <si>
+    <t>IO_propValve_s7_0</t>
+  </si>
+  <si>
+    <t>IO_propValve_s7_1</t>
+  </si>
+  <si>
+    <t>IO_propValve_s7_2</t>
+  </si>
+  <si>
+    <t>IO_propValve_s8_0</t>
+  </si>
+  <si>
+    <t>IO_propValve_s8_1</t>
+  </si>
+  <si>
+    <t>IO_propValve_s8_2</t>
+  </si>
+  <si>
+    <t>IO_propValve_s9_0</t>
+  </si>
+  <si>
+    <t>IO_propValve_s9_1</t>
+  </si>
+  <si>
+    <t>IO_propValve_s9_2</t>
+  </si>
+  <si>
+    <t>D28102</t>
+  </si>
+  <si>
+    <t>D28104</t>
+  </si>
+  <si>
+    <t>D28106</t>
+  </si>
+  <si>
+    <t>D28108</t>
+  </si>
+  <si>
+    <t>D28122</t>
+  </si>
+  <si>
+    <t>D28124</t>
+  </si>
+  <si>
+    <t>D28126</t>
+  </si>
+  <si>
+    <t>D28128</t>
+  </si>
+  <si>
+    <t>D28142</t>
+  </si>
+  <si>
+    <t>D28144</t>
+  </si>
+  <si>
+    <t>D28146</t>
+  </si>
+  <si>
+    <t>D28148</t>
+  </si>
+  <si>
+    <t>D28162</t>
+  </si>
+  <si>
+    <t>D28164</t>
+  </si>
+  <si>
+    <t>D28166</t>
+  </si>
+  <si>
+    <t>D28168</t>
+  </si>
+  <si>
+    <t>D28182</t>
+  </si>
+  <si>
+    <t>D28202</t>
+  </si>
+  <si>
+    <t>D28222</t>
+  </si>
+  <si>
+    <t>D28242</t>
+  </si>
+  <si>
+    <t>D28184</t>
+  </si>
+  <si>
+    <t>D28186</t>
+  </si>
+  <si>
+    <t>D28188</t>
+  </si>
+  <si>
+    <t>D28204</t>
+  </si>
+  <si>
+    <t>D28206</t>
+  </si>
+  <si>
+    <t>D28208</t>
+  </si>
+  <si>
+    <t>D28224</t>
+  </si>
+  <si>
+    <t>D28226</t>
+  </si>
+  <si>
+    <t>D28228</t>
+  </si>
+  <si>
+    <t>D28244</t>
+  </si>
+  <si>
+    <t>IO_waterLevel_0</t>
+  </si>
+  <si>
+    <t>IO_waterLevel_1</t>
+  </si>
+  <si>
+    <t>IO_waterLevel_2</t>
+  </si>
+  <si>
+    <t>IO_waterLevel_3</t>
+  </si>
+  <si>
+    <t>IO_waterLevel_4</t>
+  </si>
+  <si>
+    <t>IO_waterLevel_5</t>
+  </si>
+  <si>
+    <t>IO_clogSensor_0</t>
+  </si>
+  <si>
+    <t>IO_clogSensor_1</t>
+  </si>
+  <si>
+    <t>X1.0</t>
+  </si>
+  <si>
+    <t>X1.1</t>
+  </si>
+  <si>
+    <t>X1.2</t>
+  </si>
+  <si>
+    <t>X1.3</t>
+  </si>
+  <si>
+    <t>X1.4</t>
+  </si>
+  <si>
+    <t>X1.5</t>
+  </si>
+  <si>
+    <t>X1.6</t>
+  </si>
+  <si>
+    <t>X1.7</t>
+  </si>
+  <si>
+    <t>IO_solenoid_0</t>
+  </si>
+  <si>
+    <t>IO_solenoid_1</t>
+  </si>
+  <si>
+    <t>IO_solenoid_2</t>
+  </si>
+  <si>
+    <t>IO_solenoid_3</t>
+  </si>
+  <si>
+    <t>IO_pumpContact_0</t>
+  </si>
+  <si>
+    <t>IO_pumpContact_1</t>
+  </si>
+  <si>
+    <t>IO_pumpContact_2</t>
+  </si>
+  <si>
+    <t>Y1.0</t>
+  </si>
+  <si>
+    <t>Y1.1</t>
+  </si>
+  <si>
+    <t>Y1.2</t>
+  </si>
+  <si>
+    <t>Y1.3</t>
+  </si>
+  <si>
+    <t>Y1.4</t>
+  </si>
+  <si>
+    <t>Y1.5</t>
+  </si>
+  <si>
+    <t>Y1.6</t>
+  </si>
+  <si>
+    <t>D28082</t>
+  </si>
+  <si>
+    <t>D28084</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1496,7 @@
   <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2337,7 +2800,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2566,9 +3029,1125 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" t="s">
+        <v>226</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>197</v>
+      </c>
+      <c r="B18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>198</v>
+      </c>
+      <c r="B19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B20" t="s">
+        <v>229</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B21" t="s">
+        <v>230</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>201</v>
+      </c>
+      <c r="B22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>203</v>
+      </c>
+      <c r="B24" t="s">
+        <v>233</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>204</v>
+      </c>
+      <c r="B25" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>206</v>
+      </c>
+      <c r="B26" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>205</v>
+      </c>
+      <c r="B27" t="s">
+        <v>236</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>207</v>
+      </c>
+      <c r="B28" t="s">
+        <v>237</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>208</v>
+      </c>
+      <c r="B29" t="s">
+        <v>238</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>209</v>
+      </c>
+      <c r="B30" t="s">
+        <v>239</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>210</v>
+      </c>
+      <c r="B31" t="s">
+        <v>240</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>241</v>
+      </c>
+      <c r="B32" t="s">
+        <v>333</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>242</v>
+      </c>
+      <c r="B33" t="s">
+        <v>334</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>243</v>
+      </c>
+      <c r="B34" t="s">
+        <v>273</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>244</v>
+      </c>
+      <c r="B35" t="s">
+        <v>274</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>245</v>
+      </c>
+      <c r="B36" t="s">
+        <v>275</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>246</v>
+      </c>
+      <c r="B37" t="s">
+        <v>276</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>247</v>
+      </c>
+      <c r="B38" t="s">
+        <v>277</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>248</v>
+      </c>
+      <c r="B39" t="s">
+        <v>278</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>249</v>
+      </c>
+      <c r="B40" t="s">
+        <v>279</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>250</v>
+      </c>
+      <c r="B41" t="s">
+        <v>280</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>251</v>
+      </c>
+      <c r="B42" t="s">
+        <v>281</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>252</v>
+      </c>
+      <c r="B43" t="s">
+        <v>282</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>253</v>
+      </c>
+      <c r="B44" t="s">
+        <v>283</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>254</v>
+      </c>
+      <c r="B45" t="s">
+        <v>284</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>255</v>
+      </c>
+      <c r="B46" t="s">
+        <v>285</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>256</v>
+      </c>
+      <c r="B47" t="s">
+        <v>286</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>257</v>
+      </c>
+      <c r="B48" t="s">
+        <v>287</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>258</v>
+      </c>
+      <c r="B49" t="s">
+        <v>288</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>259</v>
+      </c>
+      <c r="B50" t="s">
+        <v>289</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>260</v>
+      </c>
+      <c r="B51" t="s">
+        <v>293</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>261</v>
+      </c>
+      <c r="B52" t="s">
+        <v>294</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>262</v>
+      </c>
+      <c r="B53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>263</v>
+      </c>
+      <c r="B54" t="s">
+        <v>290</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>264</v>
+      </c>
+      <c r="B55" t="s">
+        <v>296</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>265</v>
+      </c>
+      <c r="B56" t="s">
+        <v>297</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>266</v>
+      </c>
+      <c r="B57" t="s">
+        <v>298</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>267</v>
+      </c>
+      <c r="B58" t="s">
+        <v>291</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>268</v>
+      </c>
+      <c r="B59" t="s">
+        <v>299</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>269</v>
+      </c>
+      <c r="B60" t="s">
+        <v>300</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>270</v>
+      </c>
+      <c r="B61" t="s">
+        <v>301</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>271</v>
+      </c>
+      <c r="B62" t="s">
+        <v>292</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>272</v>
+      </c>
+      <c r="B63" t="s">
+        <v>302</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>303</v>
+      </c>
+      <c r="B64" t="s">
+        <v>311</v>
+      </c>
+      <c r="C64" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>304</v>
+      </c>
+      <c r="B65" t="s">
+        <v>312</v>
+      </c>
+      <c r="C65" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>305</v>
+      </c>
+      <c r="B66" t="s">
+        <v>313</v>
+      </c>
+      <c r="C66" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>306</v>
+      </c>
+      <c r="B67" t="s">
+        <v>314</v>
+      </c>
+      <c r="C67" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>307</v>
+      </c>
+      <c r="B68" t="s">
+        <v>315</v>
+      </c>
+      <c r="C68" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>308</v>
+      </c>
+      <c r="B69" t="s">
+        <v>316</v>
+      </c>
+      <c r="C69" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>309</v>
+      </c>
+      <c r="B70" t="s">
+        <v>317</v>
+      </c>
+      <c r="C70" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>310</v>
+      </c>
+      <c r="B71" t="s">
+        <v>318</v>
+      </c>
+      <c r="C71" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>319</v>
+      </c>
+      <c r="B72" t="s">
+        <v>326</v>
+      </c>
+      <c r="C72" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>320</v>
+      </c>
+      <c r="B73" t="s">
+        <v>327</v>
+      </c>
+      <c r="C73" t="s">
+        <v>3</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>321</v>
+      </c>
+      <c r="B74" t="s">
+        <v>328</v>
+      </c>
+      <c r="C74" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>322</v>
+      </c>
+      <c r="B75" t="s">
+        <v>329</v>
+      </c>
+      <c r="C75" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>323</v>
+      </c>
+      <c r="B76" t="s">
+        <v>330</v>
+      </c>
+      <c r="C76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>324</v>
+      </c>
+      <c r="B77" t="s">
+        <v>331</v>
+      </c>
+      <c r="C77" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>325</v>
+      </c>
+      <c r="B78" t="s">
+        <v>332</v>
+      </c>
+      <c r="C78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update HWConfig about Pump modbus, create relevant var in global_var_table
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5715" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5715" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="395">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1035,6 +1035,186 @@
   </si>
   <si>
     <t>D28084</t>
+  </si>
+  <si>
+    <t>MB_pump0_wStartStop</t>
+  </si>
+  <si>
+    <t>D26000</t>
+  </si>
+  <si>
+    <t>MB_pump0_wFreqCmd</t>
+  </si>
+  <si>
+    <t>D26001</t>
+  </si>
+  <si>
+    <t>MB_pump0_wInputSrc</t>
+  </si>
+  <si>
+    <t>D26010</t>
+  </si>
+  <si>
+    <t>MB_pump0_wPidFbkTerm</t>
+  </si>
+  <si>
+    <t>D26011</t>
+  </si>
+  <si>
+    <t>MB_pump0_wPidTrgtSrc</t>
+  </si>
+  <si>
+    <t>D26012</t>
+  </si>
+  <si>
+    <t>MB_pump0_wPidTrgtVal</t>
+  </si>
+  <si>
+    <t>D26013</t>
+  </si>
+  <si>
+    <t>MB_pump0_rOutputHz</t>
+  </si>
+  <si>
+    <t>D25102</t>
+  </si>
+  <si>
+    <t>MB_pump0_rAciVal</t>
+  </si>
+  <si>
+    <t>MB_pump0_rVfdStatus</t>
+  </si>
+  <si>
+    <t>MB_pump0_rVfdMode</t>
+  </si>
+  <si>
+    <t>D26005</t>
+  </si>
+  <si>
+    <t>D26002</t>
+  </si>
+  <si>
+    <t>D26003</t>
+  </si>
+  <si>
+    <t>D26004</t>
+  </si>
+  <si>
+    <t>D25112</t>
+  </si>
+  <si>
+    <t>D25001</t>
+  </si>
+  <si>
+    <t>D25135</t>
+  </si>
+  <si>
+    <t>MB_pump1_wStartStop</t>
+  </si>
+  <si>
+    <t>MB_pump1_wFreqCmd</t>
+  </si>
+  <si>
+    <t>MB_pump1_wInputSrc</t>
+  </si>
+  <si>
+    <t>MB_pump1_wPidFbkTerm</t>
+  </si>
+  <si>
+    <t>MB_pump1_wPidTrgtSrc</t>
+  </si>
+  <si>
+    <t>MB_pump1_wPidTrgtVal</t>
+  </si>
+  <si>
+    <t>MB_pump1_rOutputHz</t>
+  </si>
+  <si>
+    <t>MB_pump1_rAciVal</t>
+  </si>
+  <si>
+    <t>MB_pump1_rVfdStatus</t>
+  </si>
+  <si>
+    <t>MB_pump1_rVfdMode</t>
+  </si>
+  <si>
+    <t>MB_pump2_wStartStop</t>
+  </si>
+  <si>
+    <t>MB_pump2_wFreqCmd</t>
+  </si>
+  <si>
+    <t>MB_pump2_wInputSrc</t>
+  </si>
+  <si>
+    <t>MB_pump2_wPidFbkTerm</t>
+  </si>
+  <si>
+    <t>MB_pump2_wPidTrgtSrc</t>
+  </si>
+  <si>
+    <t>MB_pump2_wPidTrgtVal</t>
+  </si>
+  <si>
+    <t>MB_pump2_rOutputHz</t>
+  </si>
+  <si>
+    <t>MB_pump2_rAciVal</t>
+  </si>
+  <si>
+    <t>MB_pump2_rVfdStatus</t>
+  </si>
+  <si>
+    <t>MB_pump2_rVfdMode</t>
+  </si>
+  <si>
+    <t>D26015</t>
+  </si>
+  <si>
+    <t>D26014</t>
+  </si>
+  <si>
+    <t>D25302</t>
+  </si>
+  <si>
+    <t>D25312</t>
+  </si>
+  <si>
+    <t>D25201</t>
+  </si>
+  <si>
+    <t>D25335</t>
+  </si>
+  <si>
+    <t>D26020</t>
+  </si>
+  <si>
+    <t>D26021</t>
+  </si>
+  <si>
+    <t>D26025</t>
+  </si>
+  <si>
+    <t>D26022</t>
+  </si>
+  <si>
+    <t>D26023</t>
+  </si>
+  <si>
+    <t>D26024</t>
+  </si>
+  <si>
+    <t>D25502</t>
+  </si>
+  <si>
+    <t>D25512</t>
+  </si>
+  <si>
+    <t>D25401</t>
+  </si>
+  <si>
+    <t>D25535</t>
   </si>
 </sst>
 </file>
@@ -1388,7 +1568,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,7 +1597,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>25001</v>
+        <v>20001</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -1431,7 +1611,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>25002</v>
+        <v>20002</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -1445,7 +1625,7 @@
         <v>33</v>
       </c>
       <c r="B4">
-        <v>25003</v>
+        <v>20003</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1463,7 +1643,7 @@
         <v>32</v>
       </c>
       <c r="B5">
-        <v>25004</v>
+        <v>20004</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1495,9 +1675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3029,15 +3207,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
@@ -4136,6 +4314,426 @@
       </c>
       <c r="D78" s="5" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>335</v>
+      </c>
+      <c r="B79" t="s">
+        <v>336</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>337</v>
+      </c>
+      <c r="B80" t="s">
+        <v>338</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>339</v>
+      </c>
+      <c r="B81" t="s">
+        <v>352</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>341</v>
+      </c>
+      <c r="B82" t="s">
+        <v>353</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>343</v>
+      </c>
+      <c r="B83" t="s">
+        <v>354</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>345</v>
+      </c>
+      <c r="B84" t="s">
+        <v>355</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>347</v>
+      </c>
+      <c r="B85" t="s">
+        <v>348</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>349</v>
+      </c>
+      <c r="B86" t="s">
+        <v>356</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>350</v>
+      </c>
+      <c r="B87" t="s">
+        <v>357</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>351</v>
+      </c>
+      <c r="B88" t="s">
+        <v>358</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>359</v>
+      </c>
+      <c r="B89" t="s">
+        <v>340</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>360</v>
+      </c>
+      <c r="B90" t="s">
+        <v>342</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>361</v>
+      </c>
+      <c r="B91" t="s">
+        <v>379</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>362</v>
+      </c>
+      <c r="B92" t="s">
+        <v>344</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>363</v>
+      </c>
+      <c r="B93" t="s">
+        <v>346</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>364</v>
+      </c>
+      <c r="B94" t="s">
+        <v>380</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>365</v>
+      </c>
+      <c r="B95" t="s">
+        <v>381</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>366</v>
+      </c>
+      <c r="B96" t="s">
+        <v>382</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>367</v>
+      </c>
+      <c r="B97" t="s">
+        <v>383</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>368</v>
+      </c>
+      <c r="B98" t="s">
+        <v>384</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>369</v>
+      </c>
+      <c r="B99" t="s">
+        <v>385</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>370</v>
+      </c>
+      <c r="B100" t="s">
+        <v>386</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>371</v>
+      </c>
+      <c r="B101" t="s">
+        <v>387</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>372</v>
+      </c>
+      <c r="B102" t="s">
+        <v>388</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>373</v>
+      </c>
+      <c r="B103" t="s">
+        <v>389</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1</v>
+      </c>
+      <c r="D103">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>374</v>
+      </c>
+      <c r="B104" t="s">
+        <v>390</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>375</v>
+      </c>
+      <c r="B105" t="s">
+        <v>391</v>
+      </c>
+      <c r="C105" t="s">
+        <v>1</v>
+      </c>
+      <c r="D105">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>376</v>
+      </c>
+      <c r="B106" t="s">
+        <v>392</v>
+      </c>
+      <c r="C106" t="s">
+        <v>1</v>
+      </c>
+      <c r="D106">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>377</v>
+      </c>
+      <c r="B107" t="s">
+        <v>393</v>
+      </c>
+      <c r="C107" t="s">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>378</v>
+      </c>
+      <c r="B108" t="s">
+        <v>394</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1</v>
+      </c>
+      <c r="D108">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add HmiTag to IO_Mapping
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5715" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="5715" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="399">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -518,12 +518,6 @@
     <t>pump_e_FlowOrRpm</t>
   </si>
   <si>
-    <t>pump_e_FlowSetArr</t>
-  </si>
-  <si>
-    <t>pump_e_RpmSetArr</t>
-  </si>
-  <si>
     <t>pump_e_RpmValArr</t>
   </si>
   <si>
@@ -533,18 +527,12 @@
     <t>pump_h_Mode</t>
   </si>
   <si>
-    <t>pump_h_OnArr</t>
-  </si>
-  <si>
     <t>pump_h_FlowSetArr</t>
   </si>
   <si>
     <t>pump_h_RpmSetArr</t>
   </si>
   <si>
-    <t>pump_h_RpmValArr</t>
-  </si>
-  <si>
     <t>pump_h_ValveOnArr</t>
   </si>
   <si>
@@ -1236,6 +1224,9 @@
   </si>
   <si>
     <t>PUMP_LOCK_SEMI_PART</t>
+  </si>
+  <si>
+    <t>pump_h_RedundantPumpSelect</t>
   </si>
 </sst>
 </file>
@@ -2999,13 +2990,13 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
@@ -3053,44 +3044,53 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>158</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>159</v>
+      </c>
+      <c r="F4" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3098,27 +3098,30 @@
         <v>164</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>165</v>
+        <v>395</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E7" t="s">
-        <v>159</v>
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="F7" t="s">
         <v>154</v>
@@ -3126,16 +3129,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
+        <v>393</v>
+      </c>
+      <c r="E8" t="s">
+        <v>394</v>
       </c>
       <c r="F8" t="s">
         <v>154</v>
@@ -3143,16 +3146,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
       </c>
       <c r="F9" t="s">
         <v>154</v>
@@ -3160,16 +3163,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>397</v>
+        <v>158</v>
       </c>
       <c r="E10" t="s">
-        <v>398</v>
+        <v>159</v>
       </c>
       <c r="F10" t="s">
         <v>154</v>
@@ -3177,16 +3180,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>169</v>
+        <v>398</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
       </c>
       <c r="F11" t="s">
         <v>154</v>
@@ -3194,16 +3197,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>170</v>
+        <v>391</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="F12" t="s">
         <v>154</v>
@@ -3211,71 +3214,31 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>171</v>
+        <v>392</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>159</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>399</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>154</v>
-      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>395</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>154</v>
-      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>396</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" t="s">
-        <v>154</v>
-      </c>
+      <c r="D16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3286,8 +3249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3317,10 +3280,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -3331,10 +3294,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -3345,10 +3308,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -3359,10 +3322,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -3373,10 +3336,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -3387,10 +3350,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B7" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -3401,10 +3364,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B8" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -3415,10 +3378,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -3429,10 +3392,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B10" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -3443,10 +3406,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -3457,10 +3420,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B12" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -3471,10 +3434,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -3485,10 +3448,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B14" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -3499,10 +3462,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B15" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -3513,10 +3476,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B16" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
@@ -3527,10 +3490,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B17" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
@@ -3541,10 +3504,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B18" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
@@ -3555,10 +3518,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -3569,10 +3532,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B20" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -3583,10 +3546,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B21" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -3597,10 +3560,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B22" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -3611,10 +3574,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B23" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -3625,10 +3588,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B24" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
@@ -3639,10 +3602,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B25" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -3653,10 +3616,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B26" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -3667,10 +3630,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B27" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -3681,10 +3644,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B28" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
@@ -3695,10 +3658,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B29" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
@@ -3709,10 +3672,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B30" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -3723,10 +3686,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B31" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
@@ -3737,10 +3700,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B32" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
@@ -3751,10 +3714,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B33" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
@@ -3765,10 +3728,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B34" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
@@ -3779,10 +3742,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B35" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
@@ -3793,10 +3756,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B36" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -3807,10 +3770,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B37" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
@@ -3821,10 +3784,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B38" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
@@ -3835,10 +3798,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B39" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
@@ -3849,10 +3812,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B40" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
@@ -3863,10 +3826,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B41" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
@@ -3877,10 +3840,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B42" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
@@ -3891,10 +3854,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B43" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
@@ -3905,10 +3868,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B44" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C44" t="s">
         <v>1</v>
@@ -3919,10 +3882,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B45" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
@@ -3933,10 +3896,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B46" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C46" t="s">
         <v>1</v>
@@ -3947,10 +3910,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B47" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
@@ -3961,10 +3924,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B48" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
@@ -3975,10 +3938,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B49" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
@@ -3989,10 +3952,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B50" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C50" t="s">
         <v>1</v>
@@ -4003,10 +3966,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B51" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C51" t="s">
         <v>1</v>
@@ -4017,10 +3980,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B52" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
@@ -4031,10 +3994,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B53" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C53" t="s">
         <v>1</v>
@@ -4045,10 +4008,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B54" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C54" t="s">
         <v>1</v>
@@ -4059,10 +4022,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B55" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
@@ -4073,10 +4036,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B56" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C56" t="s">
         <v>1</v>
@@ -4087,10 +4050,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B57" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C57" t="s">
         <v>1</v>
@@ -4101,10 +4064,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B58" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C58" t="s">
         <v>1</v>
@@ -4115,10 +4078,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B59" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
@@ -4129,10 +4092,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B60" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
@@ -4143,10 +4106,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B61" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
@@ -4157,10 +4120,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B62" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
@@ -4171,10 +4134,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B63" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
@@ -4185,10 +4148,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B64" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C64" t="s">
         <v>3</v>
@@ -4199,10 +4162,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B65" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C65" t="s">
         <v>3</v>
@@ -4213,10 +4176,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B66" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C66" t="s">
         <v>3</v>
@@ -4227,10 +4190,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B67" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C67" t="s">
         <v>3</v>
@@ -4241,10 +4204,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B68" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C68" t="s">
         <v>3</v>
@@ -4255,10 +4218,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B69" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C69" t="s">
         <v>3</v>
@@ -4269,10 +4232,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B70" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C70" t="s">
         <v>3</v>
@@ -4283,10 +4246,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B71" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C71" t="s">
         <v>3</v>
@@ -4297,10 +4260,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B72" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C72" t="s">
         <v>3</v>
@@ -4311,10 +4274,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B73" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C73" t="s">
         <v>3</v>
@@ -4325,10 +4288,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B74" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C74" t="s">
         <v>3</v>
@@ -4339,10 +4302,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B75" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C75" t="s">
         <v>3</v>
@@ -4353,10 +4316,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B76" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C76" t="s">
         <v>3</v>
@@ -4367,10 +4330,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B77" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C77" t="s">
         <v>3</v>
@@ -4381,10 +4344,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B78" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C78" t="s">
         <v>3</v>
@@ -4395,10 +4358,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B79" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
@@ -4409,402 +4372,411 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>333</v>
+      </c>
+      <c r="B80" t="s">
+        <v>334</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>335</v>
+      </c>
+      <c r="B81" t="s">
+        <v>348</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>337</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B82" t="s">
+        <v>349</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>339</v>
+      </c>
+      <c r="B83" t="s">
+        <v>350</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>341</v>
+      </c>
+      <c r="B84" t="s">
+        <v>351</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>343</v>
+      </c>
+      <c r="B85" t="s">
+        <v>344</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>-1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>345</v>
+      </c>
+      <c r="B86" t="s">
+        <v>352</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>346</v>
+      </c>
+      <c r="B87" t="s">
+        <v>353</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>347</v>
+      </c>
+      <c r="B88" t="s">
+        <v>354</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>355</v>
+      </c>
+      <c r="B89" t="s">
+        <v>336</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>356</v>
+      </c>
+      <c r="B90" t="s">
         <v>338</v>
       </c>
-      <c r="C80" t="s">
-        <v>1</v>
-      </c>
-      <c r="D80">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>339</v>
-      </c>
-      <c r="B81" t="s">
-        <v>352</v>
-      </c>
-      <c r="C81" t="s">
-        <v>1</v>
-      </c>
-      <c r="D81">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>341</v>
-      </c>
-      <c r="B82" t="s">
-        <v>353</v>
-      </c>
-      <c r="C82" t="s">
-        <v>1</v>
-      </c>
-      <c r="D82">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>343</v>
-      </c>
-      <c r="B83" t="s">
-        <v>354</v>
-      </c>
-      <c r="C83" t="s">
-        <v>1</v>
-      </c>
-      <c r="D83">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>345</v>
-      </c>
-      <c r="B84" t="s">
-        <v>355</v>
-      </c>
-      <c r="C84" t="s">
-        <v>1</v>
-      </c>
-      <c r="D84">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>347</v>
-      </c>
-      <c r="B85" t="s">
-        <v>348</v>
-      </c>
-      <c r="C85" t="s">
-        <v>1</v>
-      </c>
-      <c r="D85">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>349</v>
-      </c>
-      <c r="B86" t="s">
-        <v>356</v>
-      </c>
-      <c r="C86" t="s">
-        <v>1</v>
-      </c>
-      <c r="D86">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>350</v>
-      </c>
-      <c r="B87" t="s">
+      <c r="C90" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>357</v>
       </c>
-      <c r="C87" t="s">
-        <v>1</v>
-      </c>
-      <c r="D87">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>351</v>
-      </c>
-      <c r="B88" t="s">
+      <c r="B91" t="s">
+        <v>375</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>358</v>
       </c>
-      <c r="C88" t="s">
-        <v>1</v>
-      </c>
-      <c r="D88">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="B92" t="s">
+        <v>340</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>359</v>
       </c>
-      <c r="B89" t="s">
-        <v>340</v>
-      </c>
-      <c r="C89" t="s">
-        <v>1</v>
-      </c>
-      <c r="D89">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="B93" t="s">
+        <v>342</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>360</v>
       </c>
-      <c r="B90" t="s">
-        <v>342</v>
-      </c>
-      <c r="C90" t="s">
-        <v>1</v>
-      </c>
-      <c r="D90">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="B94" t="s">
+        <v>376</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>361</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B95" t="s">
+        <v>377</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>-1</v>
+      </c>
+      <c r="E95" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>362</v>
+      </c>
+      <c r="B96" t="s">
+        <v>378</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>363</v>
+      </c>
+      <c r="B97" t="s">
         <v>379</v>
       </c>
-      <c r="C91" t="s">
-        <v>1</v>
-      </c>
-      <c r="D91">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>362</v>
-      </c>
-      <c r="B92" t="s">
-        <v>344</v>
-      </c>
-      <c r="C92" t="s">
-        <v>1</v>
-      </c>
-      <c r="D92">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>363</v>
-      </c>
-      <c r="B93" t="s">
-        <v>346</v>
-      </c>
-      <c r="C93" t="s">
-        <v>1</v>
-      </c>
-      <c r="D93">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="C97" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>364</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B98" t="s">
         <v>380</v>
       </c>
-      <c r="C94" t="s">
-        <v>1</v>
-      </c>
-      <c r="D94">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="C98" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>365</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B99" t="s">
         <v>381</v>
       </c>
-      <c r="C95" t="s">
-        <v>1</v>
-      </c>
-      <c r="D95">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="C99" t="s">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>366</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B100" t="s">
         <v>382</v>
       </c>
-      <c r="C96" t="s">
-        <v>1</v>
-      </c>
-      <c r="D96">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="C100" t="s">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>367</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B101" t="s">
         <v>383</v>
       </c>
-      <c r="C97" t="s">
-        <v>1</v>
-      </c>
-      <c r="D97">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="C101" t="s">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>368</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B102" t="s">
         <v>384</v>
       </c>
-      <c r="C98" t="s">
-        <v>1</v>
-      </c>
-      <c r="D98">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="C102" t="s">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>369</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B103" t="s">
         <v>385</v>
       </c>
-      <c r="C99" t="s">
-        <v>1</v>
-      </c>
-      <c r="D99">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="C103" t="s">
+        <v>1</v>
+      </c>
+      <c r="D103">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>370</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B104" t="s">
         <v>386</v>
       </c>
-      <c r="C100" t="s">
-        <v>1</v>
-      </c>
-      <c r="D100">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="C104" t="s">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>371</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B105" t="s">
         <v>387</v>
       </c>
-      <c r="C101" t="s">
-        <v>1</v>
-      </c>
-      <c r="D101">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="C105" t="s">
+        <v>1</v>
+      </c>
+      <c r="D105">
+        <v>-1</v>
+      </c>
+      <c r="E105" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>372</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B106" t="s">
         <v>388</v>
       </c>
-      <c r="C102" t="s">
-        <v>1</v>
-      </c>
-      <c r="D102">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="C106" t="s">
+        <v>1</v>
+      </c>
+      <c r="D106">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>373</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B107" t="s">
         <v>389</v>
       </c>
-      <c r="C103" t="s">
-        <v>1</v>
-      </c>
-      <c r="D103">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="C107" t="s">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>374</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B108" t="s">
         <v>390</v>
-      </c>
-      <c r="C104" t="s">
-        <v>1</v>
-      </c>
-      <c r="D104">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>375</v>
-      </c>
-      <c r="B105" t="s">
-        <v>391</v>
-      </c>
-      <c r="C105" t="s">
-        <v>1</v>
-      </c>
-      <c r="D105">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>376</v>
-      </c>
-      <c r="B106" t="s">
-        <v>392</v>
-      </c>
-      <c r="C106" t="s">
-        <v>1</v>
-      </c>
-      <c r="D106">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>377</v>
-      </c>
-      <c r="B107" t="s">
-        <v>393</v>
-      </c>
-      <c r="C107" t="s">
-        <v>1</v>
-      </c>
-      <c r="D107">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>378</v>
-      </c>
-      <c r="B108" t="s">
-        <v>394</v>
       </c>
       <c r="C108" t="s">
         <v>1</v>
@@ -4822,8 +4794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4839,10 +4811,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -4853,10 +4825,10 @@
         <v>1000</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -4865,10 +4837,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -4877,10 +4849,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -4889,7 +4861,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -4901,10 +4873,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -4913,10 +4885,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -4925,10 +4897,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -4937,7 +4909,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Integrate with HW, debug logic, adjust unit on HMI.
</commit_message>
<xml_diff>
--- a/rack_control/plc/global_variable_template.xlsx
+++ b/rack_control/plc/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="5712" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="5712" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="402">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1233,6 +1233,9 @@
   </si>
   <si>
     <t>DUMMY_BIT_FALSE</t>
+  </si>
+  <si>
+    <t>pump_flowrateFeedback</t>
   </si>
 </sst>
 </file>
@@ -2995,8 +2998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3236,8 +3239,21 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B14" t="s">
+        <v>401</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="F14" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
@@ -3256,7 +3272,7 @@
   <dimension ref="A1:E108"/>
   <sheetViews>
     <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4800,7 +4816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>